<commit_message>
LV v.0 - test ram manual mode
</commit_message>
<xml_diff>
--- a/MainBOARD/pins.xlsx
+++ b/MainBOARD/pins.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="122">
   <si>
     <t>0DIO_7</t>
   </si>
@@ -292,6 +292,105 @@
   </si>
   <si>
     <t>0DIO_5</t>
+  </si>
+  <si>
+    <t>we</t>
+  </si>
+  <si>
+    <t>sel4ramCLK</t>
+  </si>
+  <si>
+    <t>ram_address[0]</t>
+  </si>
+  <si>
+    <t>ram_address[1]</t>
+  </si>
+  <si>
+    <t>ram_address[2]</t>
+  </si>
+  <si>
+    <t>ram_address[3]</t>
+  </si>
+  <si>
+    <t>ram_address[4]</t>
+  </si>
+  <si>
+    <t>ram_address[5]</t>
+  </si>
+  <si>
+    <t>ram_address[6]</t>
+  </si>
+  <si>
+    <t>ram_address[7]</t>
+  </si>
+  <si>
+    <t>ram_address[8]</t>
+  </si>
+  <si>
+    <t>ram_address[9]</t>
+  </si>
+  <si>
+    <t>ram_address[10]</t>
+  </si>
+  <si>
+    <t>ram_address[11]</t>
+  </si>
+  <si>
+    <t>ram_address[12]</t>
+  </si>
+  <si>
+    <t>ram_address[13]</t>
+  </si>
+  <si>
+    <t>inpCLK</t>
+  </si>
+  <si>
+    <t>ram_data[0]</t>
+  </si>
+  <si>
+    <t>ram_data[1]</t>
+  </si>
+  <si>
+    <t>ram_data[2]</t>
+  </si>
+  <si>
+    <t>ram_data[3]</t>
+  </si>
+  <si>
+    <t>ram_data[4]</t>
+  </si>
+  <si>
+    <t>ram_data[5]</t>
+  </si>
+  <si>
+    <t>ram_data[6]</t>
+  </si>
+  <si>
+    <t>ram_data[7]</t>
+  </si>
+  <si>
+    <t>RAM_OUT[0]</t>
+  </si>
+  <si>
+    <t>RAM_OUT[1]</t>
+  </si>
+  <si>
+    <t>RAM_OUT[2]</t>
+  </si>
+  <si>
+    <t>RAM_OUT[3]</t>
+  </si>
+  <si>
+    <t>RAM_OUT[4]</t>
+  </si>
+  <si>
+    <t>RAM_OUT[5]</t>
+  </si>
+  <si>
+    <t>RAM_OUT[6]</t>
+  </si>
+  <si>
+    <t>RAM_OUT[7]</t>
   </si>
 </sst>
 </file>
@@ -389,6 +488,9 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -406,9 +508,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -441,23 +540,23 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Таблица4" displayName="Таблица4" ref="A1:C88" totalsRowShown="0">
   <autoFilter ref="A1:C88"/>
-  <sortState ref="A2:C91">
-    <sortCondition descending="1" ref="A1:A91"/>
+  <sortState ref="A2:C88">
+    <sortCondition ref="A1:A88"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="PIN_10M02" dataDxfId="5"/>
-    <tableColumn id="2" name="BOARD_PIN" dataDxfId="3"/>
-    <tableColumn id="3" name="ASSIGNMENT" dataDxfId="4"/>
+    <tableColumn id="2" name="BOARD_PIN" dataDxfId="4"/>
+    <tableColumn id="3" name="ASSIGNMENT" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Стиль таблицы 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Таблица46" displayName="Таблица46" ref="A1:C88" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица42" displayName="Таблица42" ref="A1:C88" totalsRowShown="0">
   <autoFilter ref="A1:C88"/>
-  <sortState ref="A2:C91">
-    <sortCondition descending="1" ref="A1:A91"/>
+  <sortState ref="A2:C88">
+    <sortCondition ref="B1:B88"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="PIN_10M02" dataDxfId="2"/>
@@ -733,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J75" sqref="J75"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,388 +859,489 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>88</v>
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>140</v>
+        <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="D3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>139</v>
+        <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="D4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>138</v>
+        <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>86</v>
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>137</v>
+        <v>7</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>85</v>
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>129</v>
+        <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>83</v>
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>128</v>
+        <v>9</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>82</v>
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="D8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>127</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>81</v>
+        <v>10</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="D9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>126</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>84</v>
+        <v>19</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>125</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>80</v>
+        <v>21</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="D11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>124</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>79</v>
+        <v>23</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>123</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>83</v>
+        <v>24</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="D13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>117</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>78</v>
+        <v>25</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="D14"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>116</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>114</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>73</v>
+        <v>27</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="D16"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>112</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>76</v>
+        <v>28</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="D17"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>106</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>71</v>
+        <v>31</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="D18"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>105</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>75</v>
+        <v>32</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="D19"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>103</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>70</v>
+        <v>33</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="D20"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>101</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>74</v>
+        <v>39</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="D21"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>100</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>69</v>
+        <v>40</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="D22"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>99</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>72</v>
+        <v>41</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="D23"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>98</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="D24"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>53</v>
+        <v>19</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="D25"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>95</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>67</v>
+        <v>46</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="D26"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>52</v>
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="D27"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>92</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>66</v>
+        <v>48</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="D28"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>51</v>
+        <v>21</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="D29"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>90</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>65</v>
+        <v>50</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="D30"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="D31"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>88</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>64</v>
+        <v>52</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="D32"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>49</v>
+        <v>23</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="D33"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>86</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="D34"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35"/>
+        <v>24</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>84</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="D36"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D37"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D38"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D39"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D40"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D41"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D42"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D43"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D44"/>
     </row>
@@ -1156,392 +1356,392 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D46"/>
       <c r="E46" s="3"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D47"/>
       <c r="E47" s="3"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D48"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D49"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D50"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D51"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
+        <v>80</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="D52"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D53"/>
       <c r="E53" s="3"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
-        <v>59</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>38</v>
+        <v>84</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="D54"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D55"/>
       <c r="E55" s="3"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
-        <v>54</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>37</v>
+        <v>86</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D56"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D57"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
-        <v>52</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>36</v>
+        <v>88</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="D58"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D59"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
-        <v>50</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>35</v>
+        <v>90</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="D60"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="D61"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
-        <v>48</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>34</v>
+        <v>92</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="D62"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D63"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
-        <v>46</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>33</v>
+        <v>95</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="D64"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="D65"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
-        <v>42</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>32</v>
+        <v>98</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="D66"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
-        <v>41</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>15</v>
+        <v>99</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="D67"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
-        <v>40</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>31</v>
+        <v>100</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="D68"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
-        <v>39</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>14</v>
+        <v>101</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="D69"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
-        <v>33</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>30</v>
+        <v>103</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="D70"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
-        <v>32</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>13</v>
+        <v>105</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="D71"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
-        <v>31</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>29</v>
+        <v>106</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="D72"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
-        <v>28</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>12</v>
+        <v>112</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="D73"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
-        <v>27</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>28</v>
+        <v>114</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="D74"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
-        <v>26</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>11</v>
+        <v>116</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="D75"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
-        <v>25</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>27</v>
+        <v>117</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="D76"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
-        <v>24</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>10</v>
+        <v>123</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="D77"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
-        <v>23</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>26</v>
+        <v>124</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D78"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
-        <v>21</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>9</v>
+        <v>125</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="D79"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
-        <v>19</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>25</v>
+        <v>126</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="D80"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
-        <v>10</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>8</v>
+        <v>127</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="D81"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="D82"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
-        <v>8</v>
+        <v>129</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="D83"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
-        <v>7</v>
+        <v>137</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="D84"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="D85"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
-        <v>5</v>
+        <v>139</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D86"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
-        <v>4</v>
+        <v>140</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>5</v>
+        <v>87</v>
       </c>
       <c r="D87"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
-        <v>3</v>
+        <v>141</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="D88"/>
     </row>
@@ -1568,15 +1768,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A43" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1592,784 +1792,850 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>141</v>
+        <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>127</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>125</v>
+        <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>112</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>106</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
+        <v>26</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
+        <v>28</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>101</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>74</v>
+        <v>32</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>100</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>99</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>98</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>95</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>92</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>90</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>88</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>86</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
+        <v>137</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>84</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>80</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>78</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>76</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>74</v>
+        <v>138</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>70</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
-        <v>68</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C47" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>67</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>63</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>55</v>
+        <v>94</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
-        <v>61</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>54</v>
+        <v>68</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C55" s="1"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
-        <v>53</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>23</v>
+        <v>128</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
-        <v>52</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>36</v>
+        <v>127</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
-        <v>51</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>22</v>
+        <v>125</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
-        <v>50</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>35</v>
+        <v>117</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
-        <v>48</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>34</v>
+        <v>106</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
-        <v>47</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>20</v>
+        <v>103</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="C63" s="1"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
-        <v>46</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>33</v>
+        <v>100</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="C64" s="1"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
-        <v>44</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>19</v>
+        <v>98</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="C65" s="1"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
-        <v>42</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>32</v>
+        <v>95</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="C66" s="1"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
-        <v>41</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>15</v>
+        <v>92</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
-        <v>40</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>31</v>
+        <v>90</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="C68" s="1"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
-        <v>39</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>14</v>
+        <v>88</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
-        <v>32</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>13</v>
+        <v>86</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
-        <v>31</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>29</v>
+        <v>84</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
-        <v>28</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>12</v>
+        <v>80</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
-        <v>27</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>28</v>
+        <v>78</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
-        <v>26</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>11</v>
+        <v>76</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
-        <v>25</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>27</v>
+        <v>74</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="C76" s="1"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
-        <v>24</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>10</v>
+        <v>69</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="C77" s="1"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
-        <v>23</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>26</v>
+        <v>67</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C78" s="1"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
-        <v>21</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>9</v>
+        <v>63</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="C79" s="1"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
-        <v>19</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>25</v>
+        <v>61</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C80" s="1"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C81" s="1"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
-        <v>9</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>4</v>
+        <v>85</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="C82" s="1"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
-        <v>8</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>7</v>
+        <v>81</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C83" s="1"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
-        <v>7</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>3</v>
+        <v>79</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="C84" s="1"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
-        <v>6</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>6</v>
+        <v>77</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="C85" s="1"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
-        <v>5</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>2</v>
+        <v>75</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="C86" s="1"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
-        <v>4</v>
+        <v>123</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="C87" s="1"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
-        <v>3</v>
+        <v>129</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="C88" s="1"/>
     </row>

</xml_diff>

<commit_message>
LV v.2 - pll test works correct
</commit_message>
<xml_diff>
--- a/MainBOARD/pins.xlsx
+++ b/MainBOARD/pins.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All_projects\VHDL_projects\10M04SCE144C8G\TEST\MainBOARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\DIPLOM\TEST_DIPLOM_10M02_vhdl\MainBOARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="reserv_copy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="126">
   <si>
     <t>0DIO_7</t>
   </si>
@@ -297,9 +297,6 @@
     <t>we</t>
   </si>
   <si>
-    <t>sel4ramCLK</t>
-  </si>
-  <si>
     <t>ram_address[0]</t>
   </si>
   <si>
@@ -391,6 +388,21 @@
   </si>
   <si>
     <t>RAM_OUT[7]</t>
+  </si>
+  <si>
+    <t>c1_ok</t>
+  </si>
+  <si>
+    <t>c2_ok</t>
+  </si>
+  <si>
+    <t>c3_ok</t>
+  </si>
+  <si>
+    <t>c4_ok</t>
+  </si>
+  <si>
+    <t>не работал?</t>
   </si>
 </sst>
 </file>
@@ -412,12 +424,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -432,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -455,6 +473,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -556,7 +578,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица42" displayName="Таблица42" ref="A1:C88" totalsRowShown="0">
   <autoFilter ref="A1:C88"/>
   <sortState ref="A2:C88">
-    <sortCondition ref="B1:B88"/>
+    <sortCondition ref="C1:C88"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="PIN_10M02" dataDxfId="2"/>
@@ -832,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,7 +899,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="D3"/>
     </row>
@@ -889,7 +911,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4"/>
     </row>
@@ -901,7 +923,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5"/>
     </row>
@@ -913,7 +935,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6"/>
     </row>
@@ -925,7 +947,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7"/>
     </row>
@@ -937,7 +959,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D8"/>
     </row>
@@ -949,7 +971,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9"/>
     </row>
@@ -961,7 +983,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10"/>
     </row>
@@ -973,7 +995,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D11"/>
     </row>
@@ -985,7 +1007,7 @@
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12"/>
     </row>
@@ -997,7 +1019,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13"/>
     </row>
@@ -1009,7 +1031,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14"/>
     </row>
@@ -1021,7 +1043,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15"/>
     </row>
@@ -1033,7 +1055,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16"/>
     </row>
@@ -1045,7 +1067,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17"/>
     </row>
@@ -1057,7 +1079,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18"/>
     </row>
@@ -1078,7 +1100,7 @@
         <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20"/>
     </row>
@@ -1090,7 +1112,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21"/>
     </row>
@@ -1102,7 +1124,7 @@
         <v>31</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D22"/>
     </row>
@@ -1114,7 +1136,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D23"/>
     </row>
@@ -1126,7 +1148,7 @@
         <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24"/>
     </row>
@@ -1138,7 +1160,7 @@
         <v>19</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D25"/>
     </row>
@@ -1150,7 +1172,7 @@
         <v>33</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D26"/>
     </row>
@@ -1162,7 +1184,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D27"/>
     </row>
@@ -1174,7 +1196,7 @@
         <v>34</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D28"/>
     </row>
@@ -1186,7 +1208,7 @@
         <v>21</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D29"/>
     </row>
@@ -1198,7 +1220,7 @@
         <v>35</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D30"/>
     </row>
@@ -1210,7 +1232,7 @@
         <v>22</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D31"/>
     </row>
@@ -1222,7 +1244,7 @@
         <v>36</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D32"/>
     </row>
@@ -1234,7 +1256,7 @@
         <v>23</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D33"/>
     </row>
@@ -1246,7 +1268,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D34"/>
     </row>
@@ -1258,11 +1280,9 @@
         <v>24</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D35"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
@@ -1271,7 +1291,10 @@
       <c r="B36" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D36"/>
+      <c r="C36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
@@ -1280,7 +1303,10 @@
       <c r="B37" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D37"/>
+      <c r="C37" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
@@ -1289,7 +1315,10 @@
       <c r="B38" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D38"/>
+      <c r="C38" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
@@ -1298,7 +1327,10 @@
       <c r="B39" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D39"/>
+      <c r="C39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
@@ -1755,7 +1787,7 @@
       <c r="D91"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -1768,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,68 +1824,80 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>9</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>116</v>
+        <v>5</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>112</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>105</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>101</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>99</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -1863,168 +1907,180 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>141</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>140</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>139</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>126</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>124</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
+        <v>42</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>113</v>
@@ -2038,246 +2094,220 @@
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>48</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>114</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>46</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>33</v>
+        <v>3</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>42</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>110</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>40</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>108</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>33</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>31</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>104</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>27</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>102</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>25</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>23</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>99</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>19</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>97</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>4</v>
+        <v>124</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>6</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>92</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
-        <v>8</v>
+        <v>137</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>10</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5">

</xml_diff>